<commit_message>
DistanceError and Connectivity inputs finished
Fuzzy-Logic-2 or SMP2 is underway. Must test 20 flights to see how well it performs
</commit_message>
<xml_diff>
--- a/Nodes.xlsx
+++ b/Nodes.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="37">
   <si>
     <t>ID</t>
   </si>
@@ -117,6 +117,24 @@
   </si>
   <si>
     <t>Sine</t>
+  </si>
+  <si>
+    <t>Percentage</t>
+  </si>
+  <si>
+    <t>Algorithm</t>
+  </si>
+  <si>
+    <t>GMTools</t>
+  </si>
+  <si>
+    <t>The Algorithm</t>
+  </si>
+  <si>
+    <t>Michal's Algorithm</t>
+  </si>
+  <si>
+    <t>Quddus Fuzzy Logic</t>
   </si>
 </sst>
 </file>
@@ -1612,11 +1630,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2121298528"/>
-        <c:axId val="2121302176"/>
+        <c:axId val="2116492752"/>
+        <c:axId val="2116496400"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2121298528"/>
+        <c:axId val="2116492752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1673,12 +1691,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2121302176"/>
+        <c:crossAx val="2116496400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2121302176"/>
+        <c:axId val="2116496400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1735,9 +1753,317 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2121298528"/>
+        <c:crossAx val="2116492752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Algorithm Performance</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$Y$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Percentage</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$X$2:$X$5</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>GMTools</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>The Algorithm</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Michal's Algorithm</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Quddus Fuzzy Logic</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$Y$2:$Y$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>70.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>75.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>90.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>95.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="-2141501184"/>
+        <c:axId val="-2141492608"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-2141501184"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2141492608"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2141492608"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2141501184"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -1824,6 +2150,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -2321,6 +2687,509 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -2367,6 +3236,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>673100</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2638,10 +3537,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V74"/>
+  <dimension ref="A1:Y74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
+      <selection activeCell="AE26" sqref="AE26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2651,7 +3550,7 @@
     <col min="13" max="13" width="26.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -2691,8 +3590,14 @@
       <c r="V1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="X1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2747,8 +3652,14 @@
       <c r="V2">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="X2" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y2">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2788,8 +3699,15 @@
         <f t="shared" ref="S3:S66" si="2">(COS(Q3)*$V$2)+$T$2</f>
         <v>21.961946980917453</v>
       </c>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="X3" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y3">
+        <f>(15/20)*100</f>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -2829,8 +3747,14 @@
         <f t="shared" si="2"/>
         <v>21.84807753012208</v>
       </c>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="X4" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y4">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
@@ -2870,8 +3794,14 @@
         <f t="shared" si="2"/>
         <v>21.659258262890681</v>
       </c>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="X5" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y5">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
@@ -2912,7 +3842,7 @@
         <v>21.396926207859085</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
@@ -2953,7 +3883,7 @@
         <v>21.063077870366499</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6</v>
       </c>
@@ -2991,7 +3921,7 @@
         <v>20.660254037844389</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>7</v>
       </c>
@@ -3029,7 +3959,7 @@
         <v>20.191520442889917</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>8</v>
       </c>
@@ -3067,7 +3997,7 @@
         <v>19.660444431189781</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>9</v>
       </c>
@@ -3105,7 +4035,7 @@
         <v>19.071067811865476</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>10</v>
       </c>
@@ -3143,7 +4073,7 @@
         <v>18.427876096865393</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>11</v>
       </c>
@@ -3172,7 +4102,7 @@
         <v>17.735764363510462</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>12</v>
       </c>
@@ -3201,7 +4131,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>13</v>
       </c>
@@ -3230,7 +4160,7 @@
         <v>16.226182617406995</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>14</v>
       </c>

</xml_diff>